<commit_message>
Remove some cash files
</commit_message>
<xml_diff>
--- a/data/20200330/20200330_data_source.xlsx
+++ b/data/20200330/20200330_data_source.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hujin/GitHub/COVID-19/data/20200330/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4599941-F286-4C4F-ADEB-8CD695017C11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F671CD-2C07-314A-9FF8-C062FC349EBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{6CE8B240-DFED-5B43-A65D-8C709B2AC1CA}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="54">
   <si>
     <t>Data</t>
   </si>
@@ -195,24 +195,6 @@
   </si>
   <si>
     <t>Lucy. This data is not that useful -- a lot of missing entries.</t>
-  </si>
-  <si>
-    <t>More covariates that need to be included</t>
-  </si>
-  <si>
-    <t>Days since first confirmed case</t>
-  </si>
-  <si>
-    <t>3 analyses</t>
-  </si>
-  <si>
-    <t>Per state analysis in US: since demographic data is more available</t>
-  </si>
-  <si>
-    <t>Per country analysis including number of tests</t>
-  </si>
-  <si>
-    <t>Per country analysis excluding number of tests</t>
   </si>
 </sst>
 </file>
@@ -575,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41B627D5-C419-B346-A31D-F13D1DFC7D7A}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -897,36 +879,6 @@
       </c>
       <c r="E19" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>